<commit_message>
hasta aca esta todo bien, seguimos con actualizaciones de sistema
</commit_message>
<xml_diff>
--- a/data/vehiculos.xlsx
+++ b/data/vehiculos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="327">
   <si>
     <t>id</t>
   </si>
@@ -85,34 +85,37 @@
     <t>Yamaha</t>
   </si>
   <si>
+    <t>MT-0798</t>
+  </si>
+  <si>
+    <t>CB500F</t>
+  </si>
+  <si>
+    <t>Ninja 400</t>
+  </si>
+  <si>
+    <t>GSX-S750</t>
+  </si>
+  <si>
+    <t>Dominar 400</t>
+  </si>
+  <si>
+    <t>300NK</t>
+  </si>
+  <si>
+    <t>TRK 502</t>
+  </si>
+  <si>
+    <t>Duke 390</t>
+  </si>
+  <si>
+    <t>Classic 350</t>
+  </si>
+  <si>
+    <t>G310R</t>
+  </si>
+  <si>
     <t>MT-07</t>
-  </si>
-  <si>
-    <t>CB500F</t>
-  </si>
-  <si>
-    <t>Ninja 400</t>
-  </si>
-  <si>
-    <t>GSX-S750</t>
-  </si>
-  <si>
-    <t>Dominar 400</t>
-  </si>
-  <si>
-    <t>300NK</t>
-  </si>
-  <si>
-    <t>TRK 502</t>
-  </si>
-  <si>
-    <t>Duke 390</t>
-  </si>
-  <si>
-    <t>Classic 350</t>
-  </si>
-  <si>
-    <t>G310R</t>
   </si>
   <si>
     <t>2020</t>
@@ -1404,31 +1407,31 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I2">
         <v>23637</v>
       </c>
       <c r="J2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="L2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1445,28 +1448,28 @@
         <v>2023</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I3">
         <v>2567</v>
       </c>
       <c r="J3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1483,28 +1486,28 @@
         <v>2025</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I4">
         <v>2658</v>
       </c>
       <c r="J4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="K4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1521,25 +1524,25 @@
         <v>2024</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I5">
         <v>2866</v>
       </c>
       <c r="J5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1556,28 +1559,28 @@
         <v>2023</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I6">
         <v>3002</v>
       </c>
       <c r="J6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1594,28 +1597,28 @@
         <v>2025</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I7">
         <v>3159</v>
       </c>
       <c r="J7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1632,28 +1635,28 @@
         <v>2024</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I8">
         <v>3337</v>
       </c>
       <c r="J8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1670,25 +1673,25 @@
         <v>2023</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I9">
         <v>3564</v>
       </c>
       <c r="J9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1705,28 +1708,28 @@
         <v>2025</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I10">
         <v>3666</v>
       </c>
       <c r="J10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K10" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L10" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1743,28 +1746,28 @@
         <v>2024</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I11">
         <v>3804</v>
       </c>
       <c r="J11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K11" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1775,34 +1778,34 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>2023</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I12">
         <v>3998</v>
       </c>
       <c r="J12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="K12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L12" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1819,25 +1822,25 @@
         <v>2025</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I13">
         <v>4193</v>
       </c>
       <c r="J13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1854,28 +1857,28 @@
         <v>2024</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I14">
         <v>4355</v>
       </c>
       <c r="J14" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="K14" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L14" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1892,28 +1895,28 @@
         <v>2023</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I15">
         <v>4528</v>
       </c>
       <c r="J15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L15" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1930,28 +1933,28 @@
         <v>2025</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I16">
         <v>4713</v>
       </c>
       <c r="J16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K16" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L16" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1968,25 +1971,25 @@
         <v>2024</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I17">
         <v>4797</v>
       </c>
       <c r="J17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L17" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2003,28 +2006,28 @@
         <v>2023</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H18" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I18">
         <v>4991</v>
       </c>
       <c r="J18" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L18" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2041,28 +2044,28 @@
         <v>2025</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I19">
         <v>5203</v>
       </c>
       <c r="J19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L19" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2079,28 +2082,28 @@
         <v>2024</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H20" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I20">
         <v>5345</v>
       </c>
       <c r="J20" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="K20" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L20" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2117,25 +2120,25 @@
         <v>2023</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H21" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I21">
         <v>5545</v>
       </c>
       <c r="J21" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L21" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2146,34 +2149,34 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>2025</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I22">
         <v>5615</v>
       </c>
       <c r="J22" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="K22" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L22" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2190,28 +2193,28 @@
         <v>2024</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H23" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I23">
         <v>5788</v>
       </c>
       <c r="J23" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="K23" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="L23" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2228,28 +2231,28 @@
         <v>2023</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H24" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I24">
         <v>5997</v>
       </c>
       <c r="J24" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="K24" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="L24" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2266,25 +2269,25 @@
         <v>2025</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I25">
         <v>6123</v>
       </c>
       <c r="J25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L25" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2301,28 +2304,28 @@
         <v>2024</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I26">
         <v>6325</v>
       </c>
       <c r="J26" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K26" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L26" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2339,28 +2342,28 @@
         <v>2023</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G27" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H27" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I27">
         <v>6450</v>
       </c>
       <c r="J27" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="K27" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L27" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2377,28 +2380,28 @@
         <v>2025</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G28" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H28" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I28">
         <v>6678</v>
       </c>
       <c r="J28" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K28" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L28" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2415,25 +2418,25 @@
         <v>2024</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H29" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I29">
         <v>6811</v>
       </c>
       <c r="J29" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L29" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2450,28 +2453,28 @@
         <v>2023</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F30" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G30" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I30">
         <v>6986</v>
       </c>
       <c r="J30" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K30" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L30" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2488,28 +2491,28 @@
         <v>2025</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G31" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H31" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I31">
         <v>7167</v>
       </c>
       <c r="J31" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="K31" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="L31" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2520,34 +2523,34 @@
         <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D32">
         <v>2024</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F32" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I32">
         <v>7284</v>
       </c>
       <c r="J32" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K32" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2564,25 +2567,25 @@
         <v>2023</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G33" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H33" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I33">
         <v>7514</v>
       </c>
       <c r="J33" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L33" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2599,28 +2602,28 @@
         <v>2025</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H34" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I34">
         <v>7669</v>
       </c>
       <c r="J34" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K34" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L34" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2637,28 +2640,28 @@
         <v>2024</v>
       </c>
       <c r="E35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H35" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I35">
         <v>7774</v>
       </c>
       <c r="J35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K35" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L35" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2675,28 +2678,28 @@
         <v>2023</v>
       </c>
       <c r="E36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G36" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H36" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I36">
         <v>7983</v>
       </c>
       <c r="J36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K36" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L36" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2713,25 +2716,25 @@
         <v>2025</v>
       </c>
       <c r="E37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G37" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H37" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I37">
         <v>8123</v>
       </c>
       <c r="J37" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L37" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2748,28 +2751,28 @@
         <v>2024</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G38" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H38" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I38">
         <v>8325</v>
       </c>
       <c r="J38" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K38" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L38" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2786,28 +2789,28 @@
         <v>2023</v>
       </c>
       <c r="E39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H39" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I39">
         <v>8439</v>
       </c>
       <c r="J39" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K39" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L39" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2824,28 +2827,28 @@
         <v>2025</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G40" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H40" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I40">
         <v>8591</v>
       </c>
       <c r="J40" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K40" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L40" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2862,25 +2865,25 @@
         <v>2024</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G41" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H41" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I41">
         <v>8760</v>
       </c>
       <c r="J41" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L41" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2891,34 +2894,34 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D42">
         <v>2023</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G42" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H42" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I42">
         <v>8949</v>
       </c>
       <c r="J42" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K42" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="L42" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2935,28 +2938,28 @@
         <v>2025</v>
       </c>
       <c r="E43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G43" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H43" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I43">
         <v>9140</v>
       </c>
       <c r="J43" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K43" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L43" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2973,28 +2976,28 @@
         <v>2024</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G44" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H44" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I44">
         <v>9312</v>
       </c>
       <c r="J44" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K44" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L44" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -3011,25 +3014,25 @@
         <v>2023</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F45" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G45" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H45" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I45">
         <v>9490</v>
       </c>
       <c r="J45" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L45" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -3046,28 +3049,28 @@
         <v>2025</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H46" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I46">
         <v>9629</v>
       </c>
       <c r="J46" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="K46" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L46" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -3084,28 +3087,28 @@
         <v>2024</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F47" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G47" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H47" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I47">
         <v>9766</v>
       </c>
       <c r="J47" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="K47" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="L47" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3122,28 +3125,28 @@
         <v>2023</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F48" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G48" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H48" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I48">
         <v>9915</v>
       </c>
       <c r="J48" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="K48" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="L48" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3160,25 +3163,25 @@
         <v>2025</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H49" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I49">
         <v>10159</v>
       </c>
       <c r="J49" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="L49" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3195,28 +3198,28 @@
         <v>2024</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G50" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H50" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I50">
         <v>10301</v>
       </c>
       <c r="J50" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K50" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L50" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3233,28 +3236,28 @@
         <v>2023</v>
       </c>
       <c r="E51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G51" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H51" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I51">
         <v>10462</v>
       </c>
       <c r="J51" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="K51" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L51" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>